<commit_message>
Update the reporting page to include description of the Viewer and User sheets. Updated the example spreadsheet to go with the text.
</commit_message>
<xml_diff>
--- a/docs/2024-annotations/Project_Manager_Worksheets.xlsx
+++ b/docs/2024-annotations/Project_Manager_Worksheets.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="42">
   <si>
     <t>Archive X</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>Ellipses, Rectangles</t>
+  </si>
+  <si>
+    <t>XXX-129</t>
   </si>
   <si>
     <t>Creator B</t>
@@ -878,7 +881,7 @@
         <v>16</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="J10" s="15"/>
       <c r="K10" s="10" t="s">
@@ -906,7 +909,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="8" t="s">
@@ -959,10 +962,10 @@
       <c r="E13" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="12"/>
+      <c r="G13" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="13"/>
       <c r="H13" s="14" t="s">
         <v>16</v>
       </c>
@@ -996,10 +999,10 @@
       <c r="E14" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="12"/>
+      <c r="G14" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="13"/>
       <c r="H14" s="14" t="s">
         <v>16</v>
       </c>
@@ -1033,10 +1036,10 @@
       <c r="E15" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="12"/>
+      <c r="G15" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="13"/>
       <c r="H15" s="14" t="s">
         <v>16</v>
       </c>
@@ -1069,7 +1072,7 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="8" t="s">
@@ -1122,10 +1125,10 @@
       <c r="E18" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F18" s="12"/>
+      <c r="G18" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="13"/>
       <c r="H18" s="14" t="s">
         <v>16</v>
       </c>
@@ -13830,7 +13833,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="17" t="s">
@@ -13880,28 +13883,28 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D3" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="H3" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="I3" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" s="20" t="s">
-        <v>30</v>
-      </c>
       <c r="J3" s="20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
@@ -14075,13 +14078,13 @@
         <v>15</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>16</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>15</v>
@@ -14107,13 +14110,13 @@
         <v>15</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>16</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G10" s="10" t="s">
         <v>15</v>
@@ -14140,32 +14143,32 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D12" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="H12" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="I12" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="H12" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="I12" s="20" t="s">
-        <v>30</v>
-      </c>
       <c r="J12" s="20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13">
@@ -14276,32 +14279,32 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D17" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="H17" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="19" t="s">
+      <c r="I17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="G17" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="H17" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="I17" s="20" t="s">
-        <v>30</v>
-      </c>
       <c r="J17" s="20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18">
@@ -14321,7 +14324,7 @@
         <v>16</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G18" s="10" t="s">
         <v>15</v>
@@ -24101,7 +24104,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="17" t="s">
@@ -24151,28 +24154,28 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D3" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="H3" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="I3" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" s="20" t="s">
-        <v>30</v>
-      </c>
       <c r="J3" s="20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
@@ -24192,7 +24195,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>15</v>
@@ -24204,7 +24207,7 @@
         <v>16</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5">
@@ -24256,7 +24259,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>15</v>
@@ -24346,13 +24349,13 @@
         <v>15</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>16</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>15</v>
@@ -24378,13 +24381,13 @@
         <v>15</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>16</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G10" s="10" t="s">
         <v>15</v>
@@ -24411,32 +24414,32 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D12" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="H12" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="I12" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="H12" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="I12" s="20" t="s">
-        <v>30</v>
-      </c>
       <c r="J12" s="20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13">
@@ -24456,7 +24459,7 @@
         <v>16</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="G13" s="10" t="s">
         <v>15</v>
@@ -24468,7 +24471,7 @@
         <v>16</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14">
@@ -24488,7 +24491,7 @@
         <v>16</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>15</v>
@@ -24547,32 +24550,32 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D17" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="H17" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="19" t="s">
+      <c r="I17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="G17" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="H17" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="I17" s="20" t="s">
-        <v>30</v>
-      </c>
       <c r="J17" s="20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18">
@@ -24592,7 +24595,7 @@
         <v>16</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G18" s="10" t="s">
         <v>15</v>
@@ -34372,7 +34375,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="17" t="s">
@@ -34422,28 +34425,28 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D3" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="19" t="s">
+      <c r="H3" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" s="20" t="s">
-        <v>39</v>
-      </c>
       <c r="J3" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4">
@@ -34617,13 +34620,13 @@
         <v>15</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>16</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>15</v>
@@ -34649,13 +34652,13 @@
         <v>15</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>16</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G10" s="10" t="s">
         <v>15</v>
@@ -34682,32 +34685,32 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D12" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="H12" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="I12" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="H12" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="I12" s="20" t="s">
-        <v>30</v>
-      </c>
       <c r="J12" s="20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13">
@@ -34818,32 +34821,32 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D17" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="H17" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="19" t="s">
+      <c r="I17" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="G17" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="H17" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="I17" s="20" t="s">
-        <v>30</v>
-      </c>
       <c r="J17" s="20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18">
@@ -34863,7 +34866,7 @@
         <v>16</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G18" s="10" t="s">
         <v>15</v>

</xml_diff>